<commit_message>
Created even queue directed checking for left, right, forward and back
</commit_message>
<xml_diff>
--- a/xbox buttons.xlsx
+++ b/xbox buttons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Simon\GitProjects\JXbox\JXbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACF6B2D9-6C8A-4F9E-8B3B-30A7C2045F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93F10DC-0D5D-4FB1-8D6A-36DF4DAE6468}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="13520" xr2:uid="{F0A631B0-56FB-47F7-92DB-039D1B4DD66C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F0A631B0-56FB-47F7-92DB-039D1B4DD66C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -536,17 +536,19 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B13" sqref="B13:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.8203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.17578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.52734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -563,7 +565,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -580,7 +582,7 @@
         <v>-0.99</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -597,7 +599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -614,7 +616,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -631,7 +633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -648,7 +650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -665,7 +667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -682,7 +684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -699,7 +701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -716,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -733,7 +735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -750,7 +752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -767,7 +769,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -784,7 +786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -801,7 +803,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -818,7 +820,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -835,7 +837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>

</xml_diff>